<commit_message>
Update main.py design, Add data.sql
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -26,33 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
-    <t>Рік</t>
-  </si>
-  <si>
-    <t>Об'єкт</t>
-  </si>
-  <si>
-    <t>Вид діяльності</t>
-  </si>
-  <si>
-    <t>Місцезнаходження</t>
-  </si>
-  <si>
-    <t>Оксид азоту, т/рік**</t>
-  </si>
-  <si>
-    <t>Cірки діоксид, т/рік**</t>
-  </si>
-  <si>
-    <t>Оксид вуглецю, т/рік**</t>
-  </si>
-  <si>
-    <t>Мікрочастинки та волокна, т/рік**</t>
-  </si>
-  <si>
-    <t>Всього, т/рік**</t>
-  </si>
-  <si>
     <t xml:space="preserve">ТзОВ «Птахокомплекс Губин» </t>
   </si>
   <si>
@@ -81,6 +54,33 @@
   </si>
   <si>
     <t>Луцьк</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>objectName</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>no2</t>
+  </si>
+  <si>
+    <t>so2</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>microparts</t>
+  </si>
+  <si>
+    <t>summary</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,31 +474,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E2">
         <v>36.826999999999998</v>
@@ -536,13 +536,13 @@
         <v>2021</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>71.177999999999997</v>
@@ -566,13 +566,13 @@
         <v>2021</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>12.298999999999999</v>
@@ -596,13 +596,13 @@
         <v>2021</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>41.2</v>
@@ -626,13 +626,13 @@
         <v>2021</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>5.7960000000000003</v>

</xml_diff>

<commit_message>
Revert "Update main.py design, Add data.sql"
This reverts commit 0565d0b9d02b9035689b426f386f509d40459547.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -26,6 +26,33 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
+    <t>Рік</t>
+  </si>
+  <si>
+    <t>Об'єкт</t>
+  </si>
+  <si>
+    <t>Вид діяльності</t>
+  </si>
+  <si>
+    <t>Місцезнаходження</t>
+  </si>
+  <si>
+    <t>Оксид азоту, т/рік**</t>
+  </si>
+  <si>
+    <t>Cірки діоксид, т/рік**</t>
+  </si>
+  <si>
+    <t>Оксид вуглецю, т/рік**</t>
+  </si>
+  <si>
+    <t>Мікрочастинки та волокна, т/рік**</t>
+  </si>
+  <si>
+    <t>Всього, т/рік**</t>
+  </si>
+  <si>
     <t xml:space="preserve">ТзОВ «Птахокомплекс Губин» </t>
   </si>
   <si>
@@ -54,33 +81,6 @@
   </si>
   <si>
     <t>Луцьк</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>objectName</t>
-  </si>
-  <si>
-    <t>activity</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>no2</t>
-  </si>
-  <si>
-    <t>so2</t>
-  </si>
-  <si>
-    <t>co</t>
-  </si>
-  <si>
-    <t>microparts</t>
-  </si>
-  <si>
-    <t>summary</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,31 +474,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>36.826999999999998</v>
@@ -536,13 +536,13 @@
         <v>2021</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>71.177999999999997</v>
@@ -566,13 +566,13 @@
         <v>2021</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>12.298999999999999</v>
@@ -596,13 +596,13 @@
         <v>2021</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>41.2</v>
@@ -626,13 +626,13 @@
         <v>2021</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>5.7960000000000003</v>

</xml_diff>

<commit_message>
Add main.py design, Add data.sql
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -26,33 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
-    <t>Рік</t>
-  </si>
-  <si>
-    <t>Об'єкт</t>
-  </si>
-  <si>
-    <t>Вид діяльності</t>
-  </si>
-  <si>
-    <t>Місцезнаходження</t>
-  </si>
-  <si>
-    <t>Оксид азоту, т/рік**</t>
-  </si>
-  <si>
-    <t>Cірки діоксид, т/рік**</t>
-  </si>
-  <si>
-    <t>Оксид вуглецю, т/рік**</t>
-  </si>
-  <si>
-    <t>Мікрочастинки та волокна, т/рік**</t>
-  </si>
-  <si>
-    <t>Всього, т/рік**</t>
-  </si>
-  <si>
     <t xml:space="preserve">ТзОВ «Птахокомплекс Губин» </t>
   </si>
   <si>
@@ -81,6 +54,33 @@
   </si>
   <si>
     <t>Луцьк</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>objectName</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>no2</t>
+  </si>
+  <si>
+    <t>so2</t>
+  </si>
+  <si>
+    <t>co</t>
+  </si>
+  <si>
+    <t>microparts</t>
+  </si>
+  <si>
+    <t>summary</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,31 +474,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -506,13 +506,13 @@
         <v>2021</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E2">
         <v>36.826999999999998</v>
@@ -536,13 +536,13 @@
         <v>2021</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>71.177999999999997</v>
@@ -566,13 +566,13 @@
         <v>2021</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>12.298999999999999</v>
@@ -596,13 +596,13 @@
         <v>2021</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>41.2</v>
@@ -626,13 +626,13 @@
         <v>2021</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E6">
         <v>5.7960000000000003</v>

</xml_diff>

<commit_message>
Edited main.py, More data data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="19">
   <si>
     <t xml:space="preserve">ТзОВ «Птахокомплекс Губин» </t>
   </si>
@@ -116,7 +116,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,12 +129,111 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -146,33 +245,73 @@
         <color rgb="FFCCCCCC"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -453,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,184 +612,619 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="17">
         <v>2021</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="21">
+        <v>24.050999999999998</v>
+      </c>
+      <c r="F2" s="21">
+        <v>3.0110000000000001</v>
+      </c>
+      <c r="G2" s="21">
+        <v>19.43</v>
+      </c>
+      <c r="H2" s="21">
+        <v>154.1</v>
+      </c>
+      <c r="I2" s="23">
+        <f t="shared" ref="I2:I4" si="0">SUM(E2:H2)</f>
+        <v>200.59199999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6">
+        <v>188.69900000000001</v>
+      </c>
+      <c r="F3" s="6">
+        <v>76.643000000000001</v>
+      </c>
+      <c r="G3" s="6">
+        <v>187.46</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" si="0"/>
+        <v>453.70300000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>65.575000000000003</v>
+      </c>
+      <c r="F4">
+        <v>45.71</v>
+      </c>
+      <c r="G4">
+        <v>97.27</v>
+      </c>
+      <c r="H4" s="6">
+        <v>19.838999999999999</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
+        <v>228.39400000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="21">
         <v>36.826999999999998</v>
       </c>
-      <c r="F2">
+      <c r="F5" s="21">
         <v>85.876000000000005</v>
       </c>
-      <c r="G2">
+      <c r="G5" s="21">
         <v>27.25</v>
       </c>
-      <c r="H2">
+      <c r="H5" s="21">
         <v>182.68700000000001</v>
       </c>
-      <c r="I2">
-        <f>SUM(E2:H2)</f>
+      <c r="I5" s="23">
+        <f>SUM(E5:H5)</f>
         <v>332.64</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2021</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6">
         <v>71.177999999999997</v>
       </c>
-      <c r="F3">
+      <c r="F6" s="6">
         <v>80.733000000000004</v>
       </c>
-      <c r="G3">
+      <c r="G6" s="6">
         <v>220.02099999999999</v>
       </c>
-      <c r="H3">
+      <c r="H6" s="6">
         <v>6.4630000000000001</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I6" si="0">SUM(E3:H3)</f>
+      <c r="I6" s="7">
+        <f>SUM(E6:H6)</f>
         <v>378.39500000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2021</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6">
         <v>12.298999999999999</v>
       </c>
-      <c r="F4">
+      <c r="F7" s="6">
         <v>5.6479999999999997</v>
       </c>
-      <c r="G4">
+      <c r="G7" s="6">
         <v>5.6479999999999997</v>
       </c>
-      <c r="H4">
+      <c r="H7" s="6">
         <v>6.766</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
+      <c r="I7" s="7">
+        <f>SUM(E7:H7)</f>
         <v>30.360999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2021</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="8" spans="1:9" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
+      <c r="D8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6">
         <v>41.2</v>
       </c>
-      <c r="F5">
+      <c r="F8" s="6">
         <v>32.731999999999999</v>
       </c>
-      <c r="G5">
+      <c r="G8" s="6">
         <v>113.739</v>
       </c>
-      <c r="H5">
+      <c r="H8" s="6">
         <v>16.46</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
+      <c r="I8" s="7">
+        <f>SUM(E8:H8)</f>
         <v>204.131</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2021</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="9" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="15">
         <v>5.7960000000000003</v>
       </c>
-      <c r="F6">
+      <c r="F9" s="15">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G6">
+      <c r="G9" s="15">
         <v>5.2539999999999996</v>
       </c>
-      <c r="H6">
+      <c r="H9" s="15">
         <v>191.50700000000001</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
+      <c r="I9" s="16">
+        <f>SUM(E9:H9)</f>
         <v>202.56800000000001</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>2019</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="21">
+        <v>31.263999999999999</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21">
+        <v>143.559</v>
+      </c>
+      <c r="H10" s="21">
+        <v>190.458</v>
+      </c>
+      <c r="I10" s="23">
+        <f>SUM(E10:H10)</f>
+        <v>365.28100000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="6">
+        <v>108.629</v>
+      </c>
+      <c r="F11" s="6">
+        <v>87.58</v>
+      </c>
+      <c r="G11" s="6">
+        <v>236.86</v>
+      </c>
+      <c r="H11" s="6">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="I11" s="7">
+        <f>SUM(E11:H11)</f>
+        <v>437.209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6">
+        <v>12.298999999999999</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="6">
+        <v>5.6479999999999997</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6.766</v>
+      </c>
+      <c r="I12" s="7">
+        <f>SUM(E12:H12)</f>
+        <v>24.713000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6">
+        <v>41.2</v>
+      </c>
+      <c r="F13" s="6">
+        <v>32.731999999999999</v>
+      </c>
+      <c r="G13" s="6">
+        <v>113.739</v>
+      </c>
+      <c r="H13" s="6">
+        <v>16.46</v>
+      </c>
+      <c r="I13" s="10">
+        <f>SUM(E13:H13)</f>
+        <v>204.131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>2019</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="15">
+        <v>3.2130000000000001</v>
+      </c>
+      <c r="F14" s="15">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G14" s="15">
+        <v>7.2670000000000003</v>
+      </c>
+      <c r="H14" s="15">
+        <v>207.465</v>
+      </c>
+      <c r="I14" s="16">
+        <f>SUM(E14:H14)</f>
+        <v>217.989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>2018</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="21">
+        <v>6.7370000000000001</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="21">
+        <v>7.8259999999999996</v>
+      </c>
+      <c r="H15" s="21">
+        <v>8.1690000000000005</v>
+      </c>
+      <c r="I15" s="23">
+        <f>SUM(E15:H15)</f>
+        <v>22.731999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3.1859999999999999</v>
+      </c>
+      <c r="F16" s="6">
+        <v>10.474</v>
+      </c>
+      <c r="G16" s="6">
+        <v>113.58</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7">
+        <f>SUM(E16:H16)</f>
+        <v>127.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="6">
+        <v>11.3</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="6">
+        <v>5.6479999999999997</v>
+      </c>
+      <c r="H17" s="6">
+        <v>5.88</v>
+      </c>
+      <c r="I17" s="7">
+        <f>SUM(E17:H17)</f>
+        <v>22.827999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="6">
+        <v>3.1859999999999999</v>
+      </c>
+      <c r="F18" s="6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G18" s="6">
+        <v>7.4210000000000003</v>
+      </c>
+      <c r="H18" s="6">
+        <v>368.75799999999998</v>
+      </c>
+      <c r="I18" s="7">
+        <f>SUM(E18:H18)</f>
+        <v>379.40799999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>2017.0357142857099</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="21">
+        <v>6.7370000000000001</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="21">
+        <v>7.8259999999999996</v>
+      </c>
+      <c r="H19" s="21">
+        <v>8.1690000000000005</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" ref="I19:I21" si="1">SUM(E19:H19)</f>
+        <v>22.731999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2017.0357142857099</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="6">
+        <v>3.1859999999999999</v>
+      </c>
+      <c r="F20" s="6">
+        <v>10.474</v>
+      </c>
+      <c r="G20" s="6">
+        <v>113.58</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7">
+        <f t="shared" si="1"/>
+        <v>127.24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>2017.0357142857099</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="15">
+        <v>11.3</v>
+      </c>
+      <c r="F21" s="27"/>
+      <c r="G21" s="15">
+        <v>5.6479999999999997</v>
+      </c>
+      <c r="H21" s="15">
+        <v>5.88</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="1"/>
+        <v>22.827999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>